<commit_message>
revised based on reviewer's comments
</commit_message>
<xml_diff>
--- a/data-raw/response_burden_scheme.xlsx
+++ b/data-raw/response_burden_scheme.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\daniehei\github\responseRateAnalysis\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC59A81E-CE99-49C4-A3DE-159BC306C106}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D356652E-CBA7-4DDC-B0C3-18DBB4F23A48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="11800" xr2:uid="{8408F874-BD1B-468E-813C-BCA83B39B1E5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17325" xr2:uid="{8408F874-BD1B-468E-813C-BCA83B39B1E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,15 +60,9 @@
     <t>Answer to sub-questions of up to 5 words</t>
   </si>
   <si>
-    <t>a) Rsponse to half-open question with less than 8 possibilities</t>
-  </si>
-  <si>
     <t>b) Response to half-open question with at least 8 possibilities</t>
   </si>
   <si>
-    <t>Answer to sub-question of up to 2 lines</t>
-  </si>
-  <si>
     <t>Answer to "please specify"</t>
   </si>
   <si>
@@ -109,6 +103,12 @@
   </si>
   <si>
     <t xml:space="preserve">    Per response category on a showcard</t>
+  </si>
+  <si>
+    <t>Answer to sub-questions of up to 2 lines</t>
+  </si>
+  <si>
+    <t>a) Response to half-open question with less than 8 possibilities</t>
   </si>
 </sst>
 </file>
@@ -463,15 +463,15 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -487,15 +487,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -503,7 +503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -511,7 +511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -519,7 +519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -527,7 +527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -535,7 +535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -543,7 +543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -551,15 +551,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -567,129 +567,129 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>11</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>12</v>
       </c>
       <c r="B16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B19">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B20">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B21">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B24">
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B25">
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B27">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B28">
         <v>1</v>

</xml_diff>